<commit_message>
feat: agregar agrupación por user_id y session_id con conteo de usuarios únicos por ruta - nuevos KPIs de agrupación: rutas populares, distribución, concentración y diversidad
</commit_message>
<xml_diff>
--- a/CursorAI/RouteAnalysys/data/export/resultados_kpis.xlsx
+++ b/CursorAI/RouteAnalysys/data/export/resultados_kpis.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,7 +483,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>66.66666666666666</v>
+        <v>60</v>
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
@@ -500,7 +500,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3.666666666666667</v>
+        <v>3.6</v>
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
@@ -534,7 +534,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>66.66666666666666</v>
+        <v>60</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -571,7 +571,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1.09861228866811</v>
+        <v>1.054920167986144</v>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
@@ -588,9 +588,9 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>1. session_start: 1 veces (33.3%)
-2. start_checkout: 1 veces (33.3%)
-3. first_visit: 1 veces (33.3%)</t>
+          <t>1. session_start: 2 veces (40.0%)
+2. start_checkout: 2 veces (40.0%)
+3. first_visit: 1 veces (20.0%)</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
@@ -608,9 +608,9 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>1. begin_checkout: 1 veces (33.3%)
-2. purchase_GA4: 1 veces (33.3%)
-3. first_visit: 1 veces (33.3%)</t>
+          <t>1. begin_checkout: 2 veces (40.0%)
+2. purchase_GA4: 2 veces (40.0%)
+3. first_visit: 1 veces (20.0%)</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
@@ -627,7 +627,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>18.18181818181818</v>
+        <v>16.66666666666666</v>
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr">
@@ -644,7 +644,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>66.66666666666666</v>
+        <v>60</v>
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr">
@@ -661,7 +661,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.4714045207910317</v>
+        <v>0.4898979485566356</v>
       </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr">
@@ -679,7 +679,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>1. begin_checkout: 3 veces (100.0%)</t>
+          <t>1. begin_checkout: 5 veces (100.0%)</t>
         </is>
       </c>
       <c r="C14" t="inlineStr"/>
@@ -709,8 +709,8 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>1. begin_checkout: 1 veces (50.0%)
-2. first_visit: 1 veces (50.0%)</t>
+          <t>1. begin_checkout: 2 veces (66.7%)
+2. first_visit: 1 veces (33.3%)</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -733,11 +733,11 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>1. first_visit: 3 veces (27.3%)
-2. begin_checkout: 3 veces (27.3%)
-3. purchase_GA4: 3 veces (27.3%)
-4. session_start: 1 veces (9.1%)
-5. start_checkout: 1 veces (9.1%)</t>
+          <t>1. begin_checkout: 5 veces (27.8%)
+2. purchase_GA4: 5 veces (27.8%)
+3. first_visit: 4 veces (22.2%)
+4. session_start: 2 veces (11.1%)
+5. start_checkout: 2 veces (11.1%)</t>
         </is>
       </c>
       <c r="C17" t="inlineStr"/>
@@ -756,14 +756,14 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>1. session_start → first_visit: 1 veces (12.5%)
-2. first_visit → begin_checkout: 1 veces (12.5%)
-3. start_checkout → begin_checkout: 1 veces (12.5%)
-4. begin_checkout → purchase_GA4: 1 veces (12.5%)
-5. purchase_GA4 → purchase_GA4: 1 veces (12.5%)
-6. first_visit → purchase_GA4: 1 veces (12.5%)
-7. purchase_GA4 → begin_checkout: 1 veces (12.5%)
-8. begin_checkout → first_visit: 1 veces (12.5%)</t>
+          <t>1. session_start → first_visit: 2 veces (15.4%)
+2. first_visit → begin_checkout: 2 veces (15.4%)
+3. start_checkout → begin_checkout: 2 veces (15.4%)
+4. begin_checkout → purchase_GA4: 2 veces (15.4%)
+5. purchase_GA4 → purchase_GA4: 2 veces (15.4%)
+6. first_visit → purchase_GA4: 1 veces (7.7%)
+7. purchase_GA4 → begin_checkout: 1 veces (7.7%)
+8. begin_checkout → first_visit: 1 veces (7.7%)</t>
         </is>
       </c>
       <c r="C18" t="inlineStr"/>
@@ -781,7 +781,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>50</v>
+        <v>33.33333333333333</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -802,7 +802,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>50</v>
+        <v>33.33333333333333</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -823,7 +823,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>33.33333333333333</v>
+        <v>20</v>
       </c>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr">
@@ -857,7 +857,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>66.66666666666666</v>
+        <v>60</v>
       </c>
       <c r="C23" t="inlineStr"/>
       <c r="D23" t="inlineStr">
@@ -901,7 +901,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -922,7 +922,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -943,7 +943,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>1.5</v>
+        <v>1.666666666666667</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -977,6 +977,78 @@
   Interpretación: Si el resultado es 2.5, en promedio hay 2-3 eventos entre conversiones sucesivas.</t>
         </is>
       </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Rutas más populares por usuarios únicos</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>1.  1 session_start - 1 first_visit - 1 begin_checkou... (1 usuarios únicos, 50.0%)
+2. first_visit - 3 purchase_GA4 - 1 begin_checkout@ -... (1 usuarios únicos, 50.0%)
+3. start_checkout - 1 begin_checkout@ - 1 purchase_GA... (1 usuarios únicos, 50.0%)</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr"/>
+      <c r="D29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Distribución de usuarios por ruta</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Distribución de usuarios por ruta:
+    - Media: 1.00 usuarios
+    - Mediana: 1.00 usuarios
+    - Máximo: 1 usuarios
+    - Mínimo: 1 usuarios
+    - Desviación estándar: 0.00 usuarios</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr"/>
+      <c r="D30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Rutas con alta concentración de usuarios</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Rutas que concentran más del 10% de usuarios (0 usuarios):
+-  1 session_start - 1 first_visit - 1 begin_checkou... (1 usuarios, 50.0%)
+- first_visit - 3 purchase_GA4 - 1 begin_checkout@ -... (1 usuarios, 50.0%)
+- start_checkout - 1 begin_checkout@ - 1 purchase_GA... (1 usuarios, 50.0%)</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr"/>
+      <c r="D31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Diversidad de rutas</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Diversidad de rutas:
+    - Total de rutas únicas: 3
+    - Total de usuarios únicos: 2
+    - Promedio de usuarios por ruta: 1.00
+    - Coeficiente de Gini (desigualdad): 0.000
+    - Ruta con más usuarios: 1 usuarios
+    - Ruta con menos usuarios: 1 usuarios</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr"/>
+      <c r="D32" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>